<commit_message>
Add Death Registration Form feature to HDS-Explorer - Set affected members during a form collection as visited members (only on DeathFormUtil missing the other ones) - Add filter to exclude member from search on MemberFilterDialog
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/death_form.xlsx
+++ b/app/src/main/res/raw/death_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26265" windowHeight="9390" tabRatio="500"/>
+    <workbookView windowWidth="28800" windowHeight="12330" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="179">
   <si>
     <t>group</t>
   </si>
@@ -238,6 +238,9 @@
     <t>5. O falecido era chefe do agregado?</t>
   </si>
   <si>
+    <t>newhead</t>
+  </si>
+  <si>
     <t>newHeadCode</t>
   </si>
   <si>
@@ -259,7 +262,7 @@
     <t>5.2. Nome do novo chefe do agregado</t>
   </si>
   <si>
-    <t>newMemberships</t>
+    <t>newRelationships</t>
   </si>
   <si>
     <t>start repeat</t>
@@ -274,6 +277,9 @@
     <t>5.4. Relação dos membros com o novo chefe do agregado</t>
   </si>
   <si>
+    <t>newheadrelat</t>
+  </si>
+  <si>
     <t>newMemberCode</t>
   </si>
   <si>
@@ -478,79 +484,61 @@
     <t>Imigração Interna</t>
   </si>
   <si>
-    <t>reasons</t>
-  </si>
-  <si>
-    <t>CAME_WITH_RELATIVES</t>
-  </si>
-  <si>
-    <t>Came with relative(s)</t>
-  </si>
-  <si>
-    <t>Veio com os parentes</t>
-  </si>
-  <si>
-    <t>FARMING</t>
-  </si>
-  <si>
-    <t>Farming</t>
-  </si>
-  <si>
-    <t>Agricultura</t>
-  </si>
-  <si>
-    <t>MARITAL_CHANGE</t>
-  </si>
-  <si>
-    <t>Change in Marital Status</t>
-  </si>
-  <si>
-    <t>Mudança de estado civil</t>
-  </si>
-  <si>
-    <t>FISHING</t>
-  </si>
-  <si>
-    <t>Fishing</t>
-  </si>
-  <si>
-    <t>Pesca</t>
-  </si>
-  <si>
-    <t>EDUCATION</t>
-  </si>
-  <si>
-    <t>Education/Scholl</t>
-  </si>
-  <si>
-    <t>Educação</t>
-  </si>
-  <si>
-    <t>HEALTH_REASON</t>
-  </si>
-  <si>
-    <t>Health Reasons</t>
-  </si>
-  <si>
-    <t>Saúde</t>
-  </si>
-  <si>
-    <t>WORK</t>
-  </si>
-  <si>
-    <t>Work</t>
-  </si>
-  <si>
-    <t>Trabalho</t>
-  </si>
-  <si>
-    <t>NEW_HOUSE</t>
-  </si>
-  <si>
-    <t>Moved to new house</t>
-  </si>
-  <si>
-    <t>Mudança para nova casa</t>
+    <t>MALARIA</t>
+  </si>
+  <si>
+    <t>Malaria</t>
+  </si>
+  <si>
+    <t>HIV_AIDS</t>
+  </si>
+  <si>
+    <t>HIV/AIDS</t>
+  </si>
+  <si>
+    <t>TB</t>
+  </si>
+  <si>
+    <t>OTHER_VB_INFECTION</t>
+  </si>
+  <si>
+    <t>Other viral/bacterial infection</t>
+  </si>
+  <si>
+    <t>Outra infecção viral/bacterial</t>
+  </si>
+  <si>
+    <t>ACCIDENT</t>
+  </si>
+  <si>
+    <t>Accident</t>
+  </si>
+  <si>
+    <t>Acidente</t>
+  </si>
+  <si>
+    <t>CRIME</t>
+  </si>
+  <si>
+    <t>Crime</t>
+  </si>
+  <si>
+    <t>AGE</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Idade avançada</t>
+  </si>
+  <si>
+    <t>UNKNOWN</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Desconhecida</t>
   </si>
   <si>
     <t>OTHER</t>
@@ -613,6 +601,15 @@
     <t>form_name::pt</t>
   </si>
   <si>
+    <t>form_version</t>
+  </si>
+  <si>
+    <t>repeat_name</t>
+  </si>
+  <si>
+    <t>xml_node_name</t>
+  </si>
+  <si>
     <t>rawDeath</t>
   </si>
   <si>
@@ -620,6 +617,9 @@
   </si>
   <si>
     <t>Registo de Óbito</t>
+  </si>
+  <si>
+    <t>rawDeathRelationship</t>
   </si>
 </sst>
 </file>
@@ -627,10 +627,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -690,8 +690,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -706,7 +744,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -714,32 +752,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -753,29 +768,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -789,11 +782,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -812,17 +819,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -852,187 +852,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1043,6 +1043,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1076,15 +1091,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1095,21 +1101,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1129,8 +1120,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1139,149 +1130,158 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1291,11 +1291,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1315,15 +1318,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1668,19 +1677,19 @@
   <sheetPr/>
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="12.9142857142857" customWidth="1"/>
+    <col min="1" max="1" width="20.5714285714286" customWidth="1"/>
     <col min="2" max="2" width="11.1428571428571" customWidth="1"/>
     <col min="3" max="3" width="14.1428571428571" customWidth="1"/>
     <col min="4" max="4" width="20.1428571428571" customWidth="1"/>
     <col min="5" max="5" width="11.7142857142857" customWidth="1"/>
-    <col min="6" max="6" width="13.5238095238095" style="13" customWidth="1"/>
-    <col min="7" max="7" width="20" style="13" customWidth="1"/>
+    <col min="6" max="6" width="13.5238095238095" style="16" customWidth="1"/>
+    <col min="7" max="7" width="20" style="16" customWidth="1"/>
     <col min="8" max="8" width="51.5714285714286" customWidth="1"/>
     <col min="9" max="9" width="55" customWidth="1"/>
     <col min="10" max="10" width="16.352380952381" customWidth="1"/>
@@ -1706,10 +1715,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="16" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1730,7 +1739,7 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="16" t="s">
         <v>13</v>
       </c>
       <c r="O1" t="s">
@@ -1743,13 +1752,13 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="17" t="s">
         <v>18</v>
       </c>
       <c r="I2" t="s">
@@ -1763,7 +1772,7 @@
       <c r="M2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="N2" s="13"/>
+      <c r="N2" s="16"/>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
@@ -1775,15 +1784,15 @@
       <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="20"/>
+      <c r="G3" s="23"/>
       <c r="H3" t="s">
         <v>21</v>
       </c>
       <c r="I3" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
       <c r="L3" t="b">
         <v>1</v>
       </c>
@@ -1801,15 +1810,15 @@
       <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="20"/>
+      <c r="G4" s="23"/>
       <c r="H4" t="s">
         <v>24</v>
       </c>
       <c r="I4" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
       <c r="L4" t="b">
         <v>1</v>
       </c>
@@ -1825,15 +1834,15 @@
       <c r="E5" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="20"/>
+      <c r="G5" s="23"/>
       <c r="H5" t="s">
         <v>28</v>
       </c>
       <c r="I5" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
       <c r="L5" t="b">
         <v>1</v>
       </c>
@@ -1846,18 +1855,18 @@
       <c r="E6" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="20"/>
+      <c r="G6" s="23"/>
       <c r="H6" t="s">
         <v>33</v>
       </c>
       <c r="I6" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
       <c r="L6" t="b">
         <v>1</v>
       </c>
@@ -1870,15 +1879,15 @@
       <c r="E7" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="20"/>
+      <c r="G7" s="23"/>
       <c r="H7" t="s">
         <v>36</v>
       </c>
       <c r="I7" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
       <c r="L7" t="b">
         <v>1</v>
       </c>
@@ -1894,18 +1903,18 @@
       <c r="E8" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="20"/>
+      <c r="G8" s="23"/>
       <c r="H8" t="s">
         <v>41</v>
       </c>
       <c r="I8" t="s">
         <v>42</v>
       </c>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
       <c r="L8" t="b">
         <v>1</v>
       </c>
@@ -1918,15 +1927,15 @@
       <c r="E9" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="20"/>
+      <c r="G9" s="23"/>
       <c r="H9" t="s">
         <v>44</v>
       </c>
       <c r="I9" t="s">
         <v>45</v>
       </c>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
       <c r="L9" t="b">
         <v>1</v>
       </c>
@@ -1942,18 +1951,18 @@
       <c r="E10" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="20"/>
+      <c r="G10" s="23"/>
       <c r="H10" t="s">
         <v>49</v>
       </c>
       <c r="I10" t="s">
         <v>50</v>
       </c>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
       <c r="L10" t="b">
         <v>1</v>
       </c>
@@ -1962,21 +1971,23 @@
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E11" t="s">
         <v>17</v>
       </c>
       <c r="H11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I11" t="s">
-        <v>53</v>
-      </c>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
+        <v>54</v>
+      </c>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
       <c r="L11" t="b">
         <v>1</v>
       </c>
@@ -1984,110 +1995,116 @@
         <v>1</v>
       </c>
       <c r="N11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="1"/>
-      <c r="D12" s="15" t="s">
+      <c r="A12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="23"/>
+      <c r="H12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" t="s">
+        <v>58</v>
+      </c>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" t="b">
+        <v>1</v>
+      </c>
+      <c r="M12" t="b">
+        <v>1</v>
+      </c>
+      <c r="N12" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="20"/>
-      <c r="H12" t="s">
-        <v>56</v>
-      </c>
-      <c r="I12" t="s">
-        <v>57</v>
-      </c>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" t="b">
-        <v>1</v>
-      </c>
-      <c r="M12" t="b">
-        <v>1</v>
-      </c>
-      <c r="N12" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="16"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="18" t="s">
+      <c r="A13" s="19"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21" t="s">
+      <c r="E13" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="F13" s="24"/>
+      <c r="G13" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="I13" s="22" t="s">
+      <c r="H13" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="O13" s="22"/>
+      <c r="I13" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="O13" s="25"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="19"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
+      <c r="A14" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
         <v>17</v>
       </c>
       <c r="H14" t="s">
+        <v>66</v>
+      </c>
+      <c r="I14" t="s">
+        <v>67</v>
+      </c>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="I14" t="s">
-        <v>65</v>
-      </c>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" t="b">
-        <v>1</v>
-      </c>
-      <c r="M14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="19"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E15" t="s">
         <v>17</v>
       </c>
       <c r="H15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I15" t="s">
-        <v>68</v>
-      </c>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
+        <v>70</v>
+      </c>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
       <c r="L15" t="b">
         <v>1</v>
       </c>
@@ -2096,69 +2113,69 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="19"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
       <c r="D16" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E16" t="s">
-        <v>70</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>73</v>
       </c>
       <c r="H16" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I16" t="s">
-        <v>73</v>
-      </c>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
+        <v>75</v>
+      </c>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
       <c r="L16" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="16"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D18" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E18" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H18" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I18" t="s">
-        <v>79</v>
-      </c>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
+        <v>81</v>
+      </c>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
       <c r="L18" t="b">
         <v>1</v>
       </c>
@@ -2168,22 +2185,22 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D19" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E19" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H19" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I19" t="s">
-        <v>83</v>
-      </c>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
+        <v>85</v>
+      </c>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
       <c r="L19" t="b">
         <v>1</v>
       </c>
@@ -2193,22 +2210,22 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D20" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E20" t="s">
         <v>17</v>
       </c>
       <c r="H20" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="I20" t="s">
-        <v>86</v>
-      </c>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
+        <v>88</v>
+      </c>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
       <c r="L20" t="b">
         <v>1</v>
       </c>
@@ -2218,23 +2235,23 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="1"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="24"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="1"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="1"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="1"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="1"/>
@@ -2282,15 +2299,16 @@
   <sheetPr/>
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="12.5714285714286" customWidth="1"/>
     <col min="2" max="2" width="25.8571428571429" style="1" customWidth="1"/>
-    <col min="3" max="4" width="22.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="26.0190476190476" customWidth="1"/>
+    <col min="4" max="4" width="22.8571428571429" customWidth="1"/>
     <col min="5" max="5" width="13.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2299,7 +2317,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -2319,10 +2337,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E2" s="1"/>
     </row>
@@ -2334,478 +2352,478 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="C4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="A5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="C5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="A6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="C6" s="3" t="s">
         <v>102</v>
       </c>
+      <c r="D6" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D7" s="6" t="s">
+      <c r="A7" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>105</v>
       </c>
+      <c r="C7" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D8" s="6" t="s">
+      <c r="A8" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>108</v>
       </c>
+      <c r="C8" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="A9" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>111</v>
       </c>
+      <c r="C9" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="A10" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>114</v>
       </c>
+      <c r="C10" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="A11" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>117</v>
       </c>
+      <c r="C11" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="A12" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>120</v>
       </c>
+      <c r="C12" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="A13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>123</v>
       </c>
+      <c r="C13" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="D14" s="6" t="s">
+      <c r="A14" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>126</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E24" s="13"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C25" t="s">
         <v>127</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="D25" t="s">
         <v>128</v>
       </c>
-      <c r="C15" t="s">
-        <v>129</v>
-      </c>
-      <c r="D15" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="D16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="D17" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="D18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="D19" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="D20" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="D21" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E25" s="13"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E26" s="13"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="E28" s="13"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="E29" s="13"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B23" s="8" t="s">
+      <c r="C30" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="D23" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="D24" t="s">
-        <v>158</v>
-      </c>
-      <c r="E24" s="9"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C25" t="s">
-        <v>125</v>
-      </c>
-      <c r="D25" t="s">
-        <v>126</v>
-      </c>
-      <c r="E25" s="9"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="E26" s="9"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="E27" s="10"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="D28" s="6" t="s">
+      <c r="D30" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="E28" s="9"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E29" s="9"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="E30" s="9"/>
+      <c r="E30" s="13"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="7"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="10"/>
+      <c r="A31" s="8"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="15"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="7"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
+      <c r="A32" s="8"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="7"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="7"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
+      <c r="A34" s="8"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="7"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
+      <c r="A35" s="8"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="7"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
+      <c r="A36" s="8"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="7"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
+      <c r="A37" s="8"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
     </row>
     <row r="39" spans="5:5">
-      <c r="E39" s="9"/>
+      <c r="E39" s="13"/>
     </row>
     <row r="40" spans="5:5">
-      <c r="E40" s="9"/>
+      <c r="E40" s="13"/>
     </row>
     <row r="41" spans="5:5">
-      <c r="E41" s="9"/>
+      <c r="E41" s="13"/>
     </row>
     <row r="42" spans="5:5">
-      <c r="E42" s="10"/>
+      <c r="E42" s="15"/>
     </row>
     <row r="43" spans="5:5">
-      <c r="E43" s="9"/>
+      <c r="E43" s="13"/>
     </row>
     <row r="44" spans="5:5">
-      <c r="E44" s="9"/>
+      <c r="E44" s="13"/>
     </row>
     <row r="45" spans="5:5">
-      <c r="E45" s="9"/>
+      <c r="E45" s="13"/>
     </row>
     <row r="46" spans="5:5">
-      <c r="E46" s="9"/>
+      <c r="E46" s="13"/>
     </row>
     <row r="47" spans="5:5">
-      <c r="E47" s="9"/>
+      <c r="E47" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2817,38 +2835,59 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="21.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="20.4285714285714" customWidth="1"/>
-    <col min="3" max="3" width="23.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="19.7428571428571" customWidth="1"/>
+    <col min="4" max="4" width="11.552380952381" customWidth="1"/>
+    <col min="5" max="5" width="14.7809523809524" customWidth="1"/>
+    <col min="6" max="6" width="20.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>176</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>177</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>178</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Add French Translation to the App and improve other trenslations - Conclude the Visit termination after marking all as non-visited - First complete HDS-Explorer Tablet Version build 210
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/death_form.xlsx
+++ b/app/src/main/res/raw/death_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12330" tabRatio="500"/>
+    <workbookView windowHeight="17670" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
             <b/>
             <sz val="9"/>
             <rFont val="Times New Roman"/>
-            <charset val="0"/>
+            <charset val="134"/>
           </rPr>
           <t>paul:</t>
         </r>
@@ -36,7 +36,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Times New Roman"/>
-            <charset val="0"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 Means get houshold resident members except member represented by memberCode
@@ -54,14 +54,14 @@
     <author>paul</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="Times New Roman"/>
-            <charset val="0"/>
+            <charset val="134"/>
           </rPr>
           <t>paul:</t>
         </r>
@@ -69,7 +69,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Times New Roman"/>
-            <charset val="0"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 The option is readonly, not choosable.
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="230">
   <si>
     <t>group</t>
   </si>
@@ -112,6 +112,9 @@
     <t>label::pt</t>
   </si>
   <si>
+    <t>label::fr</t>
+  </si>
+  <si>
     <t>default_value</t>
   </si>
   <si>
@@ -145,6 +148,9 @@
     <t>1.0. Código da Visita</t>
   </si>
   <si>
+    <t>1.0. Code de Visite</t>
+  </si>
+  <si>
     <t>memberCode</t>
   </si>
   <si>
@@ -154,6 +160,12 @@
     <t>1.1. Código do Membro</t>
   </si>
   <si>
+    <t>1.1. Code du Membre</t>
+  </si>
+  <si>
+    <t>header2</t>
+  </si>
+  <si>
     <t>memberName</t>
   </si>
   <si>
@@ -163,6 +175,9 @@
     <t>1.2. Nome completo</t>
   </si>
   <si>
+    <t xml:space="preserve">1.2. Nom et prénom </t>
+  </si>
+  <si>
     <t>deathDate</t>
   </si>
   <si>
@@ -172,7 +187,10 @@
     <t>2.1. Date of Death</t>
   </si>
   <si>
-    <t>2.1. Data da Morte?</t>
+    <t>2.1. Data da Morte</t>
+  </si>
+  <si>
+    <t>2.1. Date de Décès</t>
   </si>
   <si>
     <t>deathCause</t>
@@ -190,6 +208,9 @@
     <t>3.1. Causas da Morte</t>
   </si>
   <si>
+    <t>3.1. Causes de Décès</t>
+  </si>
+  <si>
     <t>deathCauseOther</t>
   </si>
   <si>
@@ -199,6 +220,9 @@
     <t>3.2. Especifique as causas da morte</t>
   </si>
   <si>
+    <t>3.2. Précisez les causes de décès</t>
+  </si>
+  <si>
     <t>${deathCause} = 'OTHER'</t>
   </si>
   <si>
@@ -211,7 +235,10 @@
     <t>4.1. Place of Death</t>
   </si>
   <si>
-    <t>4.1. Lugar em ocorreu a morte</t>
+    <t>4.1. Lugar onde ocorreu a morte</t>
+  </si>
+  <si>
+    <t>4.1. Lieu de décès</t>
   </si>
   <si>
     <t>deathPlaceOther</t>
@@ -223,6 +250,9 @@
     <t>4.2. Especifique o lugar onde ocorreu a morte</t>
   </si>
   <si>
+    <t>4.2. Précisez le lieu où le décès est survenu</t>
+  </si>
+  <si>
     <t>${deathPlace} = 'OTHER'</t>
   </si>
   <si>
@@ -238,6 +268,9 @@
     <t>5. O falecido era chefe do agregado?</t>
   </si>
   <si>
+    <t>5. Le défunt était-il chef de famille ?</t>
+  </si>
+  <si>
     <t>newhead</t>
   </si>
   <si>
@@ -250,6 +283,9 @@
     <t>5.1. Códido do novo chefe do agregado</t>
   </si>
   <si>
+    <t>5.1. Code du nouveau chef de famille</t>
+  </si>
+  <si>
     <t>${isHouseholdHead} = 'TRUE'</t>
   </si>
   <si>
@@ -262,6 +298,9 @@
     <t>5.2. Nome do novo chefe do agregado</t>
   </si>
   <si>
+    <t>5.2. Nom du nouveau chef de famille</t>
+  </si>
+  <si>
     <t>newRelationships</t>
   </si>
   <si>
@@ -277,6 +316,9 @@
     <t>5.4. Relação dos membros com o novo chefe do agregado</t>
   </si>
   <si>
+    <t>5.4. Relation des membres avec le nouveau chef de famille</t>
+  </si>
+  <si>
     <t>newheadrelat</t>
   </si>
   <si>
@@ -289,6 +331,9 @@
     <t>5.4.1. Código do Membro</t>
   </si>
   <si>
+    <t>5.4.1. Code du Membre</t>
+  </si>
+  <si>
     <t>newMemberName</t>
   </si>
   <si>
@@ -298,6 +343,9 @@
     <t>5.4.2. Nome do Membro</t>
   </si>
   <si>
+    <t>5.4.2. Nom du Membre</t>
+  </si>
+  <si>
     <t>newRelationshipType</t>
   </si>
   <si>
@@ -313,6 +361,9 @@
     <t>5.4.3. Relação com o novo chefe do agregado</t>
   </si>
   <si>
+    <t>5.4.3. Relation avec le nouveau chef de ménage</t>
+  </si>
+  <si>
     <t>end repeat</t>
   </si>
   <si>
@@ -328,7 +379,10 @@
     <t>6.1. Collected By Fieldworker</t>
   </si>
   <si>
-    <t>6.1. Códido do Inquiridor</t>
+    <t>6.1. Código do Inquiridor</t>
+  </si>
+  <si>
+    <t>6.1. Code de l'enquêteur</t>
   </si>
   <si>
     <t>collectedDate</t>
@@ -343,6 +397,9 @@
     <t>6.2. Data da Visita</t>
   </si>
   <si>
+    <t>6.2. Date de Collecte</t>
+  </si>
+  <si>
     <t>modules</t>
   </si>
   <si>
@@ -352,6 +409,9 @@
     <t>Acesso permitido aos Módulos</t>
   </si>
   <si>
+    <t>Accès aux Modules autorisé</t>
+  </si>
+  <si>
     <t>value</t>
   </si>
   <si>
@@ -361,12 +421,18 @@
     <t>Sim</t>
   </si>
   <si>
+    <t>Oui</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
     <t>Não</t>
   </si>
   <si>
+    <t>Non</t>
+  </si>
+  <si>
     <t>genders</t>
   </si>
   <si>
@@ -379,6 +445,9 @@
     <t>Masculino</t>
   </si>
   <si>
+    <t>Masculin</t>
+  </si>
+  <si>
     <t>F</t>
   </si>
   <si>
@@ -388,15 +457,21 @@
     <t>Feminino</t>
   </si>
   <si>
+    <t>Féminin</t>
+  </si>
+  <si>
     <t>HOH</t>
   </si>
   <si>
-    <t>Head of Household</t>
+    <t>Head of household</t>
   </si>
   <si>
     <t>Chefe do Agregado</t>
   </si>
   <si>
+    <t>Chef de ménage</t>
+  </si>
+  <si>
     <t>true</t>
   </si>
   <si>
@@ -406,7 +481,10 @@
     <t>Spouse</t>
   </si>
   <si>
-    <t>Esposo/a</t>
+    <t>Cônjuge</t>
+  </si>
+  <si>
+    <t>Conjoint</t>
   </si>
   <si>
     <t>SON</t>
@@ -418,6 +496,9 @@
     <t>Filho/Filha</t>
   </si>
   <si>
+    <t>Fils/Fille</t>
+  </si>
+  <si>
     <t>BRO</t>
   </si>
   <si>
@@ -427,6 +508,9 @@
     <t>Irmão/Irmã</t>
   </si>
   <si>
+    <t>Frère/Sœur</t>
+  </si>
+  <si>
     <t>PAR</t>
   </si>
   <si>
@@ -436,6 +520,9 @@
     <t>Pai/Mãe</t>
   </si>
   <si>
+    <t>Père/Mère</t>
+  </si>
+  <si>
     <t>GCH</t>
   </si>
   <si>
@@ -445,43 +532,58 @@
     <t>Neto/a</t>
   </si>
   <si>
+    <t>Petits-enfants</t>
+  </si>
+  <si>
     <t>NOR</t>
   </si>
   <si>
-    <t>Not Related</t>
+    <t>Not related</t>
   </si>
   <si>
     <t>Sem relação</t>
   </si>
   <si>
+    <t>Aucune relation</t>
+  </si>
+  <si>
     <t>OTH</t>
   </si>
   <si>
-    <t>Other Relative</t>
+    <t>Other relative</t>
   </si>
   <si>
     <t>Outro parente</t>
   </si>
   <si>
+    <t>Autre parent</t>
+  </si>
+  <si>
     <t>DNK</t>
   </si>
   <si>
-    <t>Don't Know</t>
+    <t>Doesn't know</t>
   </si>
   <si>
     <t>Não sabe</t>
   </si>
   <si>
+    <t>Ne sait pas</t>
+  </si>
+  <si>
     <t>migtypes</t>
   </si>
   <si>
     <t>ENT</t>
   </si>
   <si>
-    <t>Internal InMigration</t>
-  </si>
-  <si>
-    <t>Imigração Interna</t>
+    <t>Internal immigration</t>
+  </si>
+  <si>
+    <t>Imigração interna</t>
+  </si>
+  <si>
+    <t>Immigration interne</t>
   </si>
   <si>
     <t>MALARIA</t>
@@ -490,12 +592,24 @@
     <t>Malaria</t>
   </si>
   <si>
+    <t>Malária</t>
+  </si>
+  <si>
+    <t>Paludisme</t>
+  </si>
+  <si>
     <t>HIV_AIDS</t>
   </si>
   <si>
     <t>HIV/AIDS</t>
   </si>
   <si>
+    <t>HIV/SIDA</t>
+  </si>
+  <si>
+    <t>VIH/SIDA</t>
+  </si>
+  <si>
     <t>TB</t>
   </si>
   <si>
@@ -508,6 +622,9 @@
     <t>Outra infecção viral/bacterial</t>
   </si>
   <si>
+    <t>Autre infection virale/bactérienne</t>
+  </si>
+  <si>
     <t>ACCIDENT</t>
   </si>
   <si>
@@ -523,15 +640,21 @@
     <t>Crime</t>
   </si>
   <si>
+    <t>Délit</t>
+  </si>
+  <si>
     <t>AGE</t>
   </si>
   <si>
-    <t>Age</t>
+    <t>Old age</t>
   </si>
   <si>
     <t>Idade avançada</t>
   </si>
   <si>
+    <t>Âge avancé</t>
+  </si>
+  <si>
     <t>UNKNOWN</t>
   </si>
   <si>
@@ -541,6 +664,9 @@
     <t>Desconhecida</t>
   </si>
   <si>
+    <t>Inconnu</t>
+  </si>
+  <si>
     <t>OTHER</t>
   </si>
   <si>
@@ -550,9 +676,15 @@
     <t>Outra</t>
   </si>
   <si>
+    <t>Autre</t>
+  </si>
+  <si>
     <t>DONT_KNOW</t>
   </si>
   <si>
+    <t>Don't know</t>
+  </si>
+  <si>
     <t>HOME</t>
   </si>
   <si>
@@ -562,6 +694,9 @@
     <t>Em casa</t>
   </si>
   <si>
+    <t>À la maison</t>
+  </si>
+  <si>
     <t>HOSPITAL</t>
   </si>
   <si>
@@ -571,13 +706,19 @@
     <t>No Hospital</t>
   </si>
   <si>
+    <t>À l'hôpital</t>
+  </si>
+  <si>
     <t>HEALTH_CENTER</t>
   </si>
   <si>
     <t>Health Centre or Clinic</t>
   </si>
   <si>
-    <t>No centro de saude ou Clinica</t>
+    <t>No centro de saúde ou Clínica</t>
+  </si>
+  <si>
+    <t>Au centre de santé ou à la clinique</t>
   </si>
   <si>
     <t>TRAD_HEALER</t>
@@ -589,9 +730,15 @@
     <t>Na casa do curandeiro</t>
   </si>
   <si>
+    <t>Dans la maison du guérisseur</t>
+  </si>
+  <si>
     <t>Outro local</t>
   </si>
   <si>
+    <t>Autre endroit</t>
+  </si>
+  <si>
     <t>form_id</t>
   </si>
   <si>
@@ -601,6 +748,9 @@
     <t>form_name::pt</t>
   </si>
   <si>
+    <t>form_name::fr</t>
+  </si>
+  <si>
     <t>form_version</t>
   </si>
   <si>
@@ -617,6 +767,9 @@
   </si>
   <si>
     <t>Registo de Óbito</t>
+  </si>
+  <si>
+    <t>Enregistrement des décès</t>
   </si>
   <si>
     <t>rawDeathRelationship</t>
@@ -628,11 +781,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="28">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -642,16 +795,11 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="0"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
@@ -675,14 +823,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -692,7 +832,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -706,15 +869,23 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -728,6 +899,14 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Arial"/>
@@ -735,24 +914,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -774,17 +944,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -797,47 +974,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="Times New Roman"/>
-      <charset val="0"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
-      <charset val="0"/>
+      <charset val="134"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -846,7 +994,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.5"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -858,7 +1024,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -870,19 +1060,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -894,7 +1072,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -906,37 +1144,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -948,25 +1162,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -978,12 +1180,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -994,55 +1190,37 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1057,6 +1235,24 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1077,6 +1273,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -1091,21 +1302,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1116,222 +1312,203 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1340,27 +1517,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1675,31 +1846,32 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="20.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="11.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="14.1428571428571" customWidth="1"/>
-    <col min="4" max="4" width="20.1428571428571" customWidth="1"/>
-    <col min="5" max="5" width="11.7142857142857" customWidth="1"/>
-    <col min="6" max="6" width="13.5238095238095" style="16" customWidth="1"/>
-    <col min="7" max="7" width="20" style="16" customWidth="1"/>
-    <col min="8" max="8" width="51.5714285714286" customWidth="1"/>
+    <col min="1" max="1" width="20.5428571428571" customWidth="1"/>
+    <col min="2" max="2" width="11.1809523809524" customWidth="1"/>
+    <col min="3" max="3" width="14.1809523809524" customWidth="1"/>
+    <col min="4" max="4" width="20.1809523809524" customWidth="1"/>
+    <col min="5" max="5" width="11.7238095238095" customWidth="1"/>
+    <col min="6" max="6" width="13.5428571428571" style="20" customWidth="1"/>
+    <col min="7" max="7" width="20" style="20" customWidth="1"/>
+    <col min="8" max="8" width="51.5428571428571" customWidth="1"/>
     <col min="9" max="9" width="55" customWidth="1"/>
-    <col min="10" max="10" width="16.352380952381" customWidth="1"/>
-    <col min="11" max="11" width="13.5333333333333" customWidth="1"/>
-    <col min="12" max="12" width="9.28571428571429" customWidth="1"/>
-    <col min="14" max="14" width="31" customWidth="1"/>
-    <col min="15" max="15" width="13.4285714285714" customWidth="1"/>
+    <col min="10" max="10" width="40.0857142857143" customWidth="1"/>
+    <col min="11" max="11" width="16.2666666666667" customWidth="1"/>
+    <col min="12" max="12" width="13.5428571428571" customWidth="1"/>
+    <col min="13" max="13" width="9.26666666666667" customWidth="1"/>
+    <col min="15" max="15" width="31" customWidth="1"/>
+    <col min="16" max="16" width="13.4571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1715,10 +1887,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="20" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1727,7 +1899,7 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="13" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -1739,519 +1911,567 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="20" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="17" t="s">
+      <c r="D2" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="E2" s="21" t="s">
         <v>18</v>
       </c>
+      <c r="H2" s="21" t="s">
+        <v>19</v>
+      </c>
       <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>21</v>
+      </c>
       <c r="K2" s="1"/>
-      <c r="L2" s="1" t="b">
-        <v>1</v>
-      </c>
+      <c r="L2" s="1"/>
       <c r="M2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="N2" s="16"/>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2" s="20"/>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="23"/>
+        <v>18</v>
+      </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" t="b">
-        <v>1</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
       <c r="M3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="N3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="23"/>
+        <v>18</v>
+      </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="I4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" t="b">
-        <v>1</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
       <c r="M4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" ht="13" customHeight="1" spans="1:12">
+      <c r="N4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" ht="13" customHeight="1" spans="1:13">
       <c r="A5" s="1"/>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="23"/>
+        <v>32</v>
+      </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="I5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" t="b">
+        <v>34</v>
+      </c>
+      <c r="J5" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6" s="1"/>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="23"/>
+        <v>37</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>38</v>
+      </c>
       <c r="H6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="I6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" t="b">
+        <v>40</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" s="1"/>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="23"/>
+        <v>18</v>
+      </c>
       <c r="H7" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="I7" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" t="b">
+        <v>44</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" t="b">
         <v>1</v>
       </c>
-      <c r="N7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="O7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="1"/>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="23"/>
+        <v>37</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>48</v>
+      </c>
       <c r="H8" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="I8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-      <c r="L8" t="b">
+        <v>50</v>
+      </c>
+      <c r="J8" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15">
       <c r="A9" s="1"/>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="23"/>
+        <v>18</v>
+      </c>
       <c r="H9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="I9" t="s">
-        <v>45</v>
-      </c>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" t="b">
+        <v>54</v>
+      </c>
+      <c r="J9" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" t="b">
         <v>1</v>
       </c>
-      <c r="N9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="O9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="1"/>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" s="23"/>
+        <v>37</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>58</v>
+      </c>
       <c r="H10" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="I10" t="s">
-        <v>50</v>
-      </c>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" t="b">
-        <v>1</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
       <c r="M10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="N10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H11" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="I11" t="s">
-        <v>54</v>
-      </c>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" t="b">
-        <v>1</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="J11" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
       <c r="M11" t="b">
         <v>1</v>
       </c>
-      <c r="N11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="N11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="23"/>
+        <v>62</v>
+      </c>
+      <c r="D12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="20"/>
       <c r="H12" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="I12" t="s">
-        <v>58</v>
-      </c>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" t="b">
-        <v>1</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="J12" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
       <c r="M12" t="b">
         <v>1</v>
       </c>
-      <c r="N12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" s="19"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="H13" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="I13" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="25" t="b">
+      <c r="N12" t="b">
         <v>1</v>
       </c>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="O13" s="25"/>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
+      <c r="O12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="22"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="H13" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="I13" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="J13" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="P13" s="26"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="D14" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H14" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I14" t="s">
-        <v>67</v>
-      </c>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" t="b">
-        <v>1</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="J14" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
       <c r="M14" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
+      <c r="N14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H15" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="I15" t="s">
-        <v>70</v>
-      </c>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" t="b">
-        <v>1</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="J15" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
       <c r="M15" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="22"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
+      <c r="N15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="1"/>
       <c r="D16" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="E16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" t="s">
+        <v>90</v>
+      </c>
+      <c r="I16" t="s">
+        <v>91</v>
+      </c>
+      <c r="J16" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+      <c r="M16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="22"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="H16" t="s">
-        <v>74</v>
-      </c>
-      <c r="I16" t="s">
-        <v>75</v>
-      </c>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
-      <c r="A17" s="19"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
+      <c r="E17" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
       <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="1" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="D18" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="E18" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="H18" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="I18" t="s">
-        <v>81</v>
-      </c>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27"/>
-      <c r="L18" t="b">
-        <v>1</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="J18" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
       <c r="M18" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="N18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="1" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="D19" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="E19" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="H19" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="I19" t="s">
-        <v>85</v>
-      </c>
-      <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
-      <c r="L19" t="b">
-        <v>1</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="J19" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
       <c r="M19" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="N19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="D20" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="E20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H20" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="I20" t="s">
-        <v>88</v>
-      </c>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-      <c r="L20" t="b">
-        <v>1</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="J20" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="K20" s="29"/>
+      <c r="L20" s="29"/>
       <c r="M20" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="N20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="1"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="1"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="27"/>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="1"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="27"/>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="1"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="1"/>
@@ -2297,27 +2517,28 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.18095238095238" defaultRowHeight="12.75" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="12.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="25.8571428571429" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.0190476190476" customWidth="1"/>
-    <col min="4" max="4" width="22.8571428571429" customWidth="1"/>
-    <col min="5" max="5" width="13.1428571428571" customWidth="1"/>
+    <col min="1" max="1" width="12.5428571428571" customWidth="1"/>
+    <col min="2" max="2" width="25.8190476190476" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="4" width="28.5428571428571" customWidth="1"/>
+    <col min="5" max="5" width="26.2666666666667" customWidth="1"/>
+    <col min="6" max="6" width="13.1809523809524" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -2325,505 +2546,611 @@
       <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="E1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B2" s="1" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5">
+        <v>111</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5">
+        <v>114</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5">
+        <v>119</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>99</v>
+        <v>122</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5">
+        <v>123</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>127</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="5" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>132</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="5" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>108</v>
+        <v>134</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>136</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="5" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>111</v>
+        <v>138</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>140</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="5" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>114</v>
+        <v>142</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>144</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="5" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>117</v>
+        <v>146</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>118</v>
+        <v>147</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>148</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="5" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>121</v>
+        <v>151</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>152</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="5" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>123</v>
+        <v>154</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>124</v>
+        <v>155</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>156</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="5" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>126</v>
+        <v>158</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>160</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>129</v>
+        <v>162</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>130</v>
+        <v>163</v>
       </c>
       <c r="C15" t="s">
-        <v>131</v>
+        <v>164</v>
       </c>
       <c r="D15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>165</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="8" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>133</v>
+        <v>167</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>169</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="8" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>135</v>
+        <v>171</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>136</v>
+        <v>172</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>173</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="8" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>137</v>
+        <v>175</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>137</v>
+        <v>175</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>175</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="8" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>138</v>
+        <v>176</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>139</v>
+        <v>177</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>178</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="8" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>141</v>
+        <v>180</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>142</v>
+        <v>181</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>182</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="8" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>144</v>
+        <v>183</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>145</v>
+        <v>184</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>184</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="8" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>147</v>
+        <v>187</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>188</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="8" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>149</v>
+        <v>190</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>150</v>
+        <v>191</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>192</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="8" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>152</v>
+        <v>194</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>153</v>
+        <v>195</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="E24" s="13"/>
-    </row>
-    <row r="25" spans="1:5">
+        <v>196</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="F24" s="12"/>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="8" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>155</v>
+        <v>198</v>
       </c>
       <c r="C25" t="s">
-        <v>127</v>
+        <v>199</v>
       </c>
       <c r="D25" t="s">
-        <v>128</v>
-      </c>
-      <c r="E25" s="13"/>
-    </row>
-    <row r="26" spans="1:5">
+        <v>160</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="F25" s="12"/>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="5" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>156</v>
+        <v>200</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>157</v>
+        <v>201</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="E26" s="13"/>
-    </row>
-    <row r="27" spans="1:5">
+        <v>202</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="5" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>159</v>
+        <v>204</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>160</v>
+        <v>205</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="E27" s="15"/>
-    </row>
-    <row r="28" spans="1:5">
+        <v>206</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="F27" s="10"/>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="5" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>162</v>
+        <v>208</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>163</v>
+        <v>209</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="E28" s="13"/>
-    </row>
-    <row r="29" spans="1:5">
+        <v>210</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="F28" s="12"/>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="5" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>165</v>
+        <v>212</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>166</v>
+        <v>213</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="E29" s="13"/>
-    </row>
-    <row r="30" spans="1:5">
+        <v>214</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="F29" s="12"/>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="5" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>152</v>
+        <v>194</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>153</v>
+        <v>195</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="E30" s="13"/>
-    </row>
-    <row r="31" spans="1:5">
+        <v>216</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="F30" s="12"/>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="8"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="15"/>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="B31" s="9"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="8"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="B32" s="9"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="8"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="B33" s="9"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="8"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="B34" s="9"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="8"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="B35" s="9"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="8"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="B36" s="9"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="8"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-    </row>
-    <row r="39" spans="5:5">
-      <c r="E39" s="13"/>
-    </row>
-    <row r="40" spans="5:5">
-      <c r="E40" s="13"/>
-    </row>
-    <row r="41" spans="5:5">
-      <c r="E41" s="13"/>
-    </row>
-    <row r="42" spans="5:5">
-      <c r="E42" s="15"/>
-    </row>
-    <row r="43" spans="5:5">
-      <c r="E43" s="13"/>
-    </row>
-    <row r="44" spans="5:5">
-      <c r="E44" s="13"/>
-    </row>
-    <row r="45" spans="5:5">
-      <c r="E45" s="13"/>
-    </row>
-    <row r="46" spans="5:5">
-      <c r="E46" s="13"/>
-    </row>
-    <row r="47" spans="5:5">
-      <c r="E47" s="13"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+    </row>
+    <row r="39" spans="5:6">
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+    </row>
+    <row r="40" spans="5:6">
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+    </row>
+    <row r="41" spans="5:6">
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+    </row>
+    <row r="42" spans="5:6">
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+    </row>
+    <row r="43" spans="5:6">
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+    </row>
+    <row r="44" spans="5:6">
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+    </row>
+    <row r="45" spans="5:6">
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+    </row>
+    <row r="46" spans="5:6">
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+    </row>
+    <row r="47" spans="5:6">
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2835,60 +3162,67 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.18095238095238" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="21.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="20.4285714285714" customWidth="1"/>
-    <col min="3" max="3" width="19.7428571428571" customWidth="1"/>
-    <col min="4" max="4" width="11.552380952381" customWidth="1"/>
-    <col min="5" max="5" width="14.7809523809524" customWidth="1"/>
-    <col min="6" max="6" width="20.5714285714286" customWidth="1"/>
+    <col min="1" max="1" width="21.7238095238095" customWidth="1"/>
+    <col min="2" max="2" width="20.4571428571429" customWidth="1"/>
+    <col min="3" max="3" width="19.7238095238095" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="5" max="5" width="11.5428571428571" customWidth="1"/>
+    <col min="6" max="6" width="14.7238095238095" customWidth="1"/>
+    <col min="7" max="7" width="20.5428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>169</v>
+        <v>218</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>170</v>
+        <v>219</v>
       </c>
       <c r="C1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D1" t="s">
-        <v>172</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>220</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>225</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>226</v>
       </c>
       <c r="C2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D2" s="2">
+        <v>227</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>178</v>
+      <c r="F2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Fix MemberFilters wasnt filtering Deaths and Outmigrations - Fix HForms validations, validate recordedDate and outcomeDate of Pregnancy Surveyllance forms - Quick Fix on Household Visit that was causing crashes when reopening visits - Update Forms questions
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/death_form.xlsx
+++ b/app/src/main/res/raw/death_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27795" windowHeight="12270" tabRatio="500"/>
+    <workbookView windowWidth="25830" windowHeight="9885" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="242">
   <si>
     <t>group</t>
   </si>
@@ -755,6 +755,18 @@
   </si>
   <si>
     <t>Dans la maison du guérisseur</t>
+  </si>
+  <si>
+    <t>PRIVATE_MAT_HOME</t>
+  </si>
+  <si>
+    <t>Private Maternity Home</t>
+  </si>
+  <si>
+    <t>Maternidade Privada</t>
+  </si>
+  <si>
+    <t>Maternité Privée</t>
   </si>
   <si>
     <t>Outro local</t>
@@ -804,10 +816,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -855,8 +867,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -869,9 +890,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -879,6 +907,52 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -892,38 +966,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -952,47 +1003,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1030,19 +1042,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1054,43 +1084,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1102,25 +1096,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1138,7 +1114,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1150,13 +1150,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1168,25 +1204,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1198,19 +1222,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1325,26 +1337,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1369,6 +1372,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1385,161 +1397,161 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1959,8 +1971,8 @@
   <sheetPr/>
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -2543,16 +2555,12 @@
       <c r="A20" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
       <c r="D20" s="21" t="s">
         <v>106</v>
       </c>
       <c r="E20" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
       <c r="H20" s="21" t="s">
         <v>108</v>
       </c>
@@ -2564,12 +2572,9 @@
       </c>
       <c r="K20" s="42"/>
       <c r="L20" s="42"/>
-      <c r="M20" s="21"/>
       <c r="N20" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="O20" s="21"/>
-      <c r="P20" s="21"/>
       <c r="Q20" s="21" t="b">
         <v>1</v>
       </c>
@@ -2578,16 +2583,12 @@
       <c r="A21" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
       <c r="D21" s="21" t="s">
         <v>109</v>
       </c>
       <c r="E21" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
       <c r="H21" s="21" t="s">
         <v>110</v>
       </c>
@@ -2599,12 +2600,9 @@
       </c>
       <c r="K21" s="42"/>
       <c r="L21" s="42"/>
-      <c r="M21" s="21"/>
       <c r="N21" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="O21" s="21"/>
-      <c r="P21" s="21"/>
       <c r="Q21" s="21" t="b">
         <v>1</v>
       </c>
@@ -2613,16 +2611,12 @@
       <c r="A22" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
       <c r="D22" s="21" t="s">
         <v>111</v>
       </c>
       <c r="E22" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
       <c r="H22" s="21" t="s">
         <v>112</v>
       </c>
@@ -2634,12 +2628,9 @@
       </c>
       <c r="K22" s="42"/>
       <c r="L22" s="42"/>
-      <c r="M22" s="21"/>
       <c r="N22" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="O22" s="21"/>
-      <c r="P22" s="21"/>
       <c r="Q22" s="21" t="b">
         <v>1</v>
       </c>
@@ -2742,10 +2733,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.18095238095238" defaultRowHeight="12.75" outlineLevelCol="5"/>
@@ -2754,7 +2745,7 @@
     <col min="2" max="2" width="25.8190476190476" style="1" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="28.5428571428571" customWidth="1"/>
-    <col min="5" max="5" width="26.2666666666667" customWidth="1"/>
+    <col min="5" max="5" width="32.8571428571429" customWidth="1"/>
     <col min="6" max="6" width="13.1809523809524" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3272,34 +3263,44 @@
         <v>49</v>
       </c>
       <c r="B30" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="F30" s="12"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C31" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="E30" s="18" t="s">
-        <v>225</v>
-      </c>
-      <c r="F30" s="12"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="8"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
+      <c r="D31" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="F31" s="12"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="8"/>
       <c r="B32" s="9"/>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="8"/>
@@ -3341,9 +3342,13 @@
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
     </row>
-    <row r="39" spans="5:6">
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
+    <row r="38" spans="1:6">
+      <c r="A38" s="8"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
     </row>
     <row r="40" spans="5:6">
       <c r="E40" s="12"/>
@@ -3354,12 +3359,12 @@
       <c r="F41" s="12"/>
     </row>
     <row r="42" spans="5:6">
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
     </row>
     <row r="43" spans="5:6">
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
     </row>
     <row r="44" spans="5:6">
       <c r="E44" s="12"/>
@@ -3376,6 +3381,10 @@
     <row r="47" spans="5:6">
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
+    </row>
+    <row r="48" spans="5:6">
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3406,39 +3415,39 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C1" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="E1" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B2" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C2" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -3447,7 +3456,7 @@
         <v>73</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Handle correctly Death/Outmigrations of Head of Households
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/death_form.xlsx
+++ b/app/src/main/res/raw/death_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25830" windowHeight="9885" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="27795" windowHeight="12240" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <author>paul</author>
   </authors>
   <commentList>
-    <comment ref="F12" authorId="0">
+    <comment ref="F13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="247">
   <si>
     <t>group</t>
   </si>
@@ -274,6 +274,18 @@
     <t>5.1. Le défunt était-il chef de famille ?</t>
   </si>
   <si>
+    <t>isLastMember</t>
+  </si>
+  <si>
+    <t>5.1.1. The Member was the last of this Household</t>
+  </si>
+  <si>
+    <t>5.1.1. O Membro era o último desta Casa</t>
+  </si>
+  <si>
+    <t>5.1.1. Le membre était le dernier de ce Ménage</t>
+  </si>
+  <si>
     <t>newhead</t>
   </si>
   <si>
@@ -289,7 +301,7 @@
     <t>5.2. Code du nouveau chef de famille</t>
   </si>
   <si>
-    <t>${isHouseholdHead} = 'TRUE'</t>
+    <t>${isHouseholdHead} = 'TRUE' and ${isLastMember} = 'false'</t>
   </si>
   <si>
     <t>newHeadName</t>
@@ -439,6 +451,9 @@
     <t>value</t>
   </si>
   <si>
+    <t>true</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -448,6 +463,9 @@
     <t>Oui</t>
   </si>
   <si>
+    <t>false</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
@@ -494,9 +512,6 @@
   </si>
   <si>
     <t>Chef de ménage</t>
-  </si>
-  <si>
-    <t>true</t>
   </si>
   <si>
     <t>SPO</t>
@@ -816,10 +831,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -867,41 +882,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -915,7 +899,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -927,9 +911,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -950,19 +934,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -980,9 +971,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -997,7 +988,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1005,6 +996,30 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1021,7 +1036,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1036,7 +1051,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1048,37 +1087,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1090,13 +1105,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1108,19 +1123,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1132,67 +1153,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1210,19 +1171,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1313,6 +1334,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1328,11 +1358,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1354,17 +1390,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -1374,24 +1399,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1410,160 +1422,172 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1609,6 +1633,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1618,11 +1643,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1632,11 +1660,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1650,7 +1681,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1969,10 +2002,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Q38"/>
+  <dimension ref="A1:Q39"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8:H9"/>
+      <selection activeCell="D10" sqref="D10:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -1982,15 +2015,15 @@
     <col min="3" max="3" width="14.1809523809524" customWidth="1"/>
     <col min="4" max="4" width="20.1809523809524" customWidth="1"/>
     <col min="5" max="5" width="11.7238095238095" customWidth="1"/>
-    <col min="6" max="6" width="13.5428571428571" style="23" customWidth="1"/>
-    <col min="7" max="7" width="20" style="23" customWidth="1"/>
+    <col min="6" max="6" width="13.5428571428571" style="25" customWidth="1"/>
+    <col min="7" max="7" width="20" style="25" customWidth="1"/>
     <col min="8" max="8" width="51.5428571428571" customWidth="1"/>
     <col min="9" max="9" width="55" customWidth="1"/>
     <col min="10" max="10" width="40.0857142857143" customWidth="1"/>
     <col min="11" max="11" width="16.2666666666667" customWidth="1"/>
     <col min="12" max="12" width="13.5428571428571" customWidth="1"/>
     <col min="13" max="13" width="9.26666666666667" customWidth="1"/>
-    <col min="15" max="15" width="31" customWidth="1"/>
+    <col min="15" max="15" width="56" customWidth="1"/>
     <col min="16" max="16" width="13.4571428571429" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2010,10 +2043,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="25" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -2022,7 +2055,7 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="14" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -2037,7 +2070,7 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="25" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
@@ -2053,19 +2086,19 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="26" t="s">
         <v>20</v>
       </c>
       <c r="I2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="15" t="s">
         <v>22</v>
       </c>
       <c r="K2" s="1"/>
@@ -2076,7 +2109,7 @@
       <c r="N2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="O2" s="23"/>
+      <c r="O2" s="25"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
@@ -2094,11 +2127,11 @@
       <c r="I3" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="37" t="s">
+      <c r="J3" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
       <c r="M3" t="b">
         <v>1</v>
       </c>
@@ -2122,11 +2155,11 @@
       <c r="I4" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="37" t="s">
+      <c r="J4" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
       <c r="M4" t="b">
         <v>1</v>
       </c>
@@ -2148,11 +2181,11 @@
       <c r="I5" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
       <c r="M5" t="b">
         <v>1</v>
       </c>
@@ -2165,7 +2198,7 @@
       <c r="E6" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="25" t="s">
         <v>39</v>
       </c>
       <c r="H6" t="s">
@@ -2174,11 +2207,11 @@
       <c r="I6" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="37" t="s">
+      <c r="J6" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
       <c r="M6" t="b">
         <v>1</v>
       </c>
@@ -2197,11 +2230,11 @@
       <c r="I7" t="s">
         <v>45</v>
       </c>
-      <c r="J7" s="37" t="s">
+      <c r="J7" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
       <c r="M7" t="b">
         <v>1</v>
       </c>
@@ -2217,7 +2250,7 @@
       <c r="E8" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="25" t="s">
         <v>49</v>
       </c>
       <c r="H8" t="s">
@@ -2226,11 +2259,11 @@
       <c r="I8" t="s">
         <v>51</v>
       </c>
-      <c r="J8" s="37" t="s">
+      <c r="J8" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
       <c r="M8" t="b">
         <v>1</v>
       </c>
@@ -2249,11 +2282,11 @@
       <c r="I9" t="s">
         <v>55</v>
       </c>
-      <c r="J9" s="37" t="s">
+      <c r="J9" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
       <c r="M9" t="b">
         <v>1</v>
       </c>
@@ -2269,7 +2302,7 @@
       <c r="E10" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="25" t="s">
         <v>59</v>
       </c>
       <c r="H10" t="s">
@@ -2278,11 +2311,11 @@
       <c r="I10" t="s">
         <v>61</v>
       </c>
-      <c r="J10" s="37" t="s">
+      <c r="J10" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
       <c r="M10" t="b">
         <v>1</v>
       </c>
@@ -2290,134 +2323,139 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="1" t="s">
+    <row r="11" s="21" customFormat="1" spans="1:17">
+      <c r="A11" s="27"/>
+      <c r="D11" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="34"/>
+      <c r="H11" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="E11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="I11" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="J11" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" t="b">
-        <v>1</v>
-      </c>
-      <c r="N11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O11" t="s">
-        <v>68</v>
+      <c r="K11" s="44"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="N11" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="21" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="23"/>
       <c r="H12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I12" t="s">
         <v>70</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="J12" s="37" t="s">
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" t="b">
+        <v>1</v>
+      </c>
+      <c r="N12" t="b">
+        <v>1</v>
+      </c>
+      <c r="O12" t="s">
         <v>72</v>
       </c>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" t="b">
-        <v>1</v>
-      </c>
-      <c r="N12" t="b">
-        <v>1</v>
-      </c>
-      <c r="O12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="25"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="27" t="s">
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="25"/>
+      <c r="H13" t="s">
         <v>74</v>
       </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31" t="s">
+      <c r="I13" t="s">
         <v>75</v>
       </c>
-      <c r="H13" s="32" t="s">
+      <c r="J13" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="I13" s="32" t="s">
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
+      <c r="M13" t="b">
+        <v>1</v>
+      </c>
+      <c r="N13" t="b">
+        <v>1</v>
+      </c>
+      <c r="O13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="J13" s="37" t="s">
+      <c r="E14" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="K13" s="39"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="P13" s="32"/>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="1" t="s">
+      <c r="F14" s="35"/>
+      <c r="G14" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="D14" t="s">
+      <c r="H14" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="E14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="I14" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="J14" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="K14" s="38"/>
-      <c r="L14" s="38"/>
-      <c r="M14" t="b">
-        <v>1</v>
-      </c>
-      <c r="N14" t="b">
-        <v>1</v>
-      </c>
+      <c r="K14" s="45"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="N14" s="36"/>
+      <c r="O14" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="P14" s="36"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D15" t="s">
         <v>84</v>
@@ -2431,11 +2469,11 @@
       <c r="I15" t="s">
         <v>86</v>
       </c>
-      <c r="J15" s="37" t="s">
+      <c r="J15" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="K15" s="38"/>
-      <c r="L15" s="38"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="42"/>
       <c r="M15" t="b">
         <v>1</v>
       </c>
@@ -2443,254 +2481,279 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="1"/>
+    <row r="16" spans="1:14">
+      <c r="A16" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="D16" t="s">
         <v>88</v>
       </c>
       <c r="E16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" t="s">
         <v>89</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="I16" t="s">
         <v>90</v>
       </c>
-      <c r="H16" t="s">
+      <c r="J16" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="I16" t="s">
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" t="b">
+        <v>1</v>
+      </c>
+      <c r="N16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="1"/>
+      <c r="D17" t="s">
         <v>92</v>
       </c>
-      <c r="J16" s="37" t="s">
+      <c r="E17" t="s">
         <v>93</v>
       </c>
-      <c r="K16" s="38"/>
-      <c r="L16" s="38"/>
-      <c r="M16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16">
-      <c r="A17" s="25"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="27" t="s">
+      <c r="F17" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="32"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="32"/>
-    </row>
-    <row r="18" s="20" customFormat="1" spans="1:14">
-      <c r="A18" s="28" t="s">
+      <c r="H17" t="s">
         <v>95</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="I17" t="s">
         <v>96</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="J17" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="20" t="s">
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
+      <c r="M17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" s="28"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="I18" s="20" t="s">
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="45"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+    </row>
+    <row r="19" s="22" customFormat="1" spans="1:14">
+      <c r="A19" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="J18" s="37" t="s">
+      <c r="D19" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="K18" s="41"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="N18" s="20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" s="21" customFormat="1" spans="1:14">
-      <c r="A19" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="D19" s="21" t="s">
+      <c r="E19" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="21" t="s">
+      <c r="I19" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="I19" s="21" t="s">
+      <c r="J19" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="J19" s="37" t="s">
+      <c r="K19" s="47"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="N19" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" s="23" customFormat="1" spans="1:14">
+      <c r="A20" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="K19" s="42"/>
-      <c r="L19" s="42"/>
-      <c r="M19" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="N19" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" s="21" customFormat="1" spans="1:17">
-      <c r="A20" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="D20" s="21" t="s">
+      <c r="E20" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="F20" s="39"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="H20" s="21" t="s">
+      <c r="I20" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="I20" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="K20" s="42"/>
-      <c r="L20" s="42"/>
-      <c r="N20" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" s="21" customFormat="1" spans="1:17">
-      <c r="A21" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="D21" s="21" t="s">
+      <c r="J20" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="E21" s="21" t="s">
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="N20" s="23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" s="23" customFormat="1" spans="1:17">
+      <c r="A21" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="I21" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="N21" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" s="23" customFormat="1" spans="1:17">
+      <c r="A22" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E22" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H21" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="I21" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="K21" s="42"/>
-      <c r="L21" s="42"/>
-      <c r="N21" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q21" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" s="21" customFormat="1" spans="1:17">
-      <c r="A22" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="E22" s="21" t="s">
+      <c r="H22" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="I22" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48"/>
+      <c r="N22" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" s="23" customFormat="1" spans="1:17">
+      <c r="A23" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E23" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H22" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="I22" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
-      <c r="N22" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" s="22" customFormat="1" spans="1:14">
-      <c r="A23" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="E23" s="22" t="s">
+      <c r="H23" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I23" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K23" s="48"/>
+      <c r="L23" s="48"/>
+      <c r="N23" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" s="24" customFormat="1" spans="1:14">
+      <c r="A24" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="I23" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="J23" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="K23" s="43"/>
-      <c r="L23" s="43"/>
-      <c r="M23" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="N23" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="1"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="38"/>
-      <c r="L24" s="38"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="I24" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="J24" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="K24" s="49"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="N24" s="24" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="1"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="38"/>
-      <c r="L25" s="38"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="1"/>
-      <c r="J26" s="38"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="38"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="42"/>
+      <c r="L26" s="42"/>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="1"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="38"/>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="J27" s="42"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="42"/>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="1"/>
+      <c r="J28" s="42"/>
+      <c r="K28" s="42"/>
+      <c r="L28" s="42"/>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="1"/>
@@ -2721,6 +2784,9 @@
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.39375" footer="0.39375"/>
@@ -2735,8 +2801,8 @@
   <sheetPr/>
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.18095238095238" defaultRowHeight="12.75" outlineLevelCol="5"/>
@@ -2754,7 +2820,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -2762,7 +2828,7 @@
       <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -2773,17 +2839,17 @@
       <c r="A2" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="1" t="b">
-        <v>1</v>
+      <c r="B2" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>120</v>
+        <v>124</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>125</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -2791,600 +2857,600 @@
       <c r="A3" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="1" t="b">
-        <v>0</v>
+      <c r="B3" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="C3" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="D3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>137</v>
-      </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>140</v>
+      <c r="A7" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>145</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>144</v>
+      <c r="A8" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>149</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>148</v>
+      <c r="A9" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>153</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>152</v>
+      <c r="A10" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>157</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>156</v>
+      <c r="A11" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>161</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>160</v>
+      <c r="A12" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>165</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>164</v>
+      <c r="A13" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>169</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>168</v>
+      <c r="A14" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>173</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="C15" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D15" t="s">
+        <v>178</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>210</v>
+      </c>
+      <c r="F24" s="13"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C25" t="s">
+        <v>212</v>
+      </c>
+      <c r="D25" t="s">
         <v>173</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E25" s="19" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="F24" s="12"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="F25" s="13"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="F26" s="13"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="F27" s="11"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="F28" s="13"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="F29" s="13"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="F30" s="13"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="D25" t="s">
-        <v>168</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="F25" s="12"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="11" t="s">
+      <c r="C31" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>211</v>
-      </c>
-      <c r="F26" s="12"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="F27" s="10"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E28" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="F28" s="12"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="F29" s="12"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="E30" s="18" t="s">
-        <v>227</v>
-      </c>
-      <c r="F30" s="12"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="E31" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="F31" s="12"/>
+      <c r="D31" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="F31" s="13"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="8"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="8"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="8"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="8"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="8"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="8"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="8"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
     </row>
     <row r="40" spans="5:6">
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
     </row>
     <row r="41" spans="5:6">
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
     </row>
     <row r="42" spans="5:6">
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
     </row>
     <row r="43" spans="5:6">
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
     </row>
     <row r="44" spans="5:6">
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
     </row>
     <row r="45" spans="5:6">
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
     </row>
     <row r="46" spans="5:6">
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
     </row>
     <row r="47" spans="5:6">
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
     </row>
     <row r="48" spans="5:6">
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3415,48 +3481,48 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="C1" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="E1" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="B2" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="C2" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Add isHouseholdBaseCodeValid to CodeGenerator Interface to easily find and validate Household prefixCode (this fixes DefaultCodeGenerator creation of prefix household codes) - Fix Death Form validation when editing (use the original head relationships to validate) - Fix External InMigration Form when editing (use correct column values) - Add check to compare previous Pregnancy Outcome dates with the new to be created on PregnancyOutcome FormUtil - Fix eddDate calculation on Pregnancy Registration Form - update and fix hforms logic
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/death_form.xlsx
+++ b/app/src/main/res/raw/death_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27795" windowHeight="12240" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="27795" windowHeight="12195" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -301,7 +301,7 @@
     <t>5.2. Code du nouveau chef de famille</t>
   </si>
   <si>
-    <t>${isHouseholdHead} = 'TRUE' and ${isLastMember} = 'false'</t>
+    <t>${isHouseholdHead} = 'true' and ${isLastMember} = 'false'</t>
   </si>
   <si>
     <t>newHeadName</t>
@@ -831,10 +831,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -874,18 +874,26 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -903,24 +911,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -934,10 +949,41 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -951,29 +997,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -988,38 +1019,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1063,7 +1063,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1075,19 +1183,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1099,151 +1243,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1343,17 +1343,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1373,26 +1382,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1408,174 +1408,174 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2004,8 +2004,8 @@
   <sheetPr/>
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:D11"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>

</xml_diff>